<commit_message>
report added, bugfixes, refactoring of qto_calculator. Still issue with by room metrics
</commit_message>
<xml_diff>
--- a/examples/all_metrics.xlsx
+++ b/examples/all_metrics.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="69" customWidth="1" min="1" max="1"/>
+    <col width="58" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="7" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>194.41</v>
+        <v>206.04</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>45756.53506390897</v>
+        <v>45757.92917207685</v>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>128.29</v>
+        <v>139.92</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="F3" s="4" t="n">
-        <v>45756.53506460374</v>
+        <v>45757.92917259506</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="F4" s="4" t="n">
-        <v>45756.53506514365</v>
+        <v>45757.92917313825</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="F5" s="4" t="n">
-        <v>45756.53506559736</v>
+        <v>45757.92917367213</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F6" s="4" t="n">
-        <v>45756.53506607129</v>
+        <v>45757.92917421139</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="F7" s="4" t="n">
-        <v>45756.53506658017</v>
+        <v>45757.92917475266</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="F8" s="4" t="n">
-        <v>45756.53506711906</v>
+        <v>45757.92917531369</v>
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="F9" s="4" t="n">
-        <v>45756.53506774243</v>
+        <v>45757.92917587478</v>
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="F10" s="4" t="n">
-        <v>45756.53506838089</v>
+        <v>45757.92917644019</v>
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="F11" s="4" t="n">
-        <v>45756.53506885933</v>
+        <v>45757.9291769701</v>
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="F12" s="4" t="n">
-        <v>45756.53506933474</v>
+        <v>45757.92917750831</v>
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="F13" s="4" t="n">
-        <v>45756.53506982393</v>
+        <v>45757.92917810478</v>
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="F14" s="4" t="n">
-        <v>45756.53507033135</v>
+        <v>45757.92917870005</v>
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
@@ -1101,7 +1101,7 @@
         </is>
       </c>
       <c r="F15" s="4" t="n">
-        <v>45756.53507084684</v>
+        <v>45757.92917921148</v>
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="F16" s="4" t="n">
-        <v>45756.53507146864</v>
+        <v>45757.92917972003</v>
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="F17" s="4" t="n">
-        <v>45756.53507206485</v>
+        <v>45757.92918024028</v>
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="F18" s="4" t="n">
-        <v>45756.53507259511</v>
+        <v>45757.92918075153</v>
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="F19" s="4" t="n">
-        <v>45756.53507312253</v>
+        <v>45757.92918126476</v>
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
@@ -1316,7 +1316,7 @@
         </is>
       </c>
       <c r="F20" s="4" t="n">
-        <v>45756.53507367509</v>
+        <v>45757.92918178374</v>
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
@@ -1359,7 +1359,7 @@
         </is>
       </c>
       <c r="F21" s="4" t="n">
-        <v>45756.53507420382</v>
+        <v>45757.92918231247</v>
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="F22" s="4" t="n">
-        <v>45756.53507476197</v>
+        <v>45757.92918294152</v>
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="F23" s="4" t="n">
-        <v>45756.53507532574</v>
+        <v>45757.92918361685</v>
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="F24" s="4" t="n">
-        <v>45756.5350759247</v>
+        <v>45757.92918429463</v>
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="F25" s="4" t="n">
-        <v>45756.53507663547</v>
+        <v>45757.92918514615</v>
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         </is>
       </c>
       <c r="F26" s="4" t="n">
-        <v>45756.53507743916</v>
+        <v>45757.92918624823</v>
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="F27" s="4" t="n">
-        <v>45756.53507819166</v>
+        <v>45757.92918752382</v>
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
@@ -1660,7 +1660,7 @@
         </is>
       </c>
       <c r="F28" s="4" t="n">
-        <v>45756.53507886611</v>
+        <v>45757.92918833147</v>
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="F29" s="4" t="n">
-        <v>45756.53507966916</v>
+        <v>45757.9291892874</v>
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
@@ -1746,7 +1746,7 @@
         </is>
       </c>
       <c r="F30" s="4" t="n">
-        <v>45756.53508046309</v>
+        <v>45757.92919024322</v>
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
@@ -1789,7 +1789,7 @@
         </is>
       </c>
       <c r="F31" s="4" t="n">
-        <v>45756.53508118071</v>
+        <v>45757.92919103338</v>
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
@@ -1835,7 +1835,7 @@
         </is>
       </c>
       <c r="F32" s="4" t="n">
-        <v>45756.5350817525</v>
+        <v>45757.92919159406</v>
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="F33" s="4" t="n">
-        <v>45756.53508232477</v>
+        <v>45757.92919212057</v>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
@@ -1921,7 +1921,7 @@
         </is>
       </c>
       <c r="F34" s="4" t="n">
-        <v>45756.53508289293</v>
+        <v>45757.92919265978</v>
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
@@ -1964,7 +1964,7 @@
         </is>
       </c>
       <c r="F35" s="4" t="n">
-        <v>45756.53508346489</v>
+        <v>45757.92919318138</v>
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="F36" s="4" t="n">
-        <v>45756.53508400843</v>
+        <v>45757.92919370004</v>
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="F37" s="4" t="n">
-        <v>45756.5350845607</v>
+        <v>45757.9291942432</v>
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="F38" s="4" t="n">
-        <v>45756.53508511382</v>
+        <v>45757.92919477019</v>
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
@@ -2141,7 +2141,7 @@
         </is>
       </c>
       <c r="F39" s="4" t="n">
-        <v>45756.53508565293</v>
+        <v>45757.92919529939</v>
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="F40" s="4" t="n">
-        <v>45756.53508621595</v>
+        <v>45757.92919583144</v>
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
@@ -2227,7 +2227,7 @@
         </is>
       </c>
       <c r="F41" s="4" t="n">
-        <v>45756.53508677301</v>
+        <v>45757.92919636455</v>
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="F42" s="4" t="n">
-        <v>45756.5350873252</v>
+        <v>45757.92919688532</v>
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
@@ -2313,7 +2313,7 @@
         </is>
       </c>
       <c r="F43" s="4" t="n">
-        <v>45756.53508788737</v>
+        <v>45757.92919740303</v>
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
@@ -2356,7 +2356,7 @@
         </is>
       </c>
       <c r="F44" s="4" t="n">
-        <v>45756.53508845247</v>
+        <v>45757.92919791688</v>
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
@@ -2399,7 +2399,7 @@
         </is>
       </c>
       <c r="F45" s="4" t="n">
-        <v>45756.53508902169</v>
+        <v>45757.92919842618</v>
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="F46" s="4" t="n">
-        <v>45756.53508959316</v>
+        <v>45757.92919893879</v>
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
@@ -2485,7 +2485,7 @@
         </is>
       </c>
       <c r="F47" s="4" t="n">
-        <v>45756.53509014367</v>
+        <v>45757.92919945589</v>
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
@@ -2528,7 +2528,7 @@
         </is>
       </c>
       <c r="F48" s="4" t="n">
-        <v>45756.53509071094</v>
+        <v>45757.92919997688</v>
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
@@ -2571,7 +2571,7 @@
         </is>
       </c>
       <c r="F49" s="4" t="n">
-        <v>45756.5350913201</v>
+        <v>45757.9292005638</v>
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
@@ -2614,7 +2614,7 @@
         </is>
       </c>
       <c r="F50" s="4" t="n">
-        <v>45756.53509192329</v>
+        <v>45757.92920118989</v>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
@@ -2657,7 +2657,7 @@
         </is>
       </c>
       <c r="F51" s="4" t="n">
-        <v>45756.5350924828</v>
+        <v>45757.92920184052</v>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
@@ -2700,7 +2700,7 @@
         </is>
       </c>
       <c r="F52" s="4" t="n">
-        <v>45756.53509299907</v>
+        <v>45757.9292024253</v>
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
@@ -2747,7 +2747,7 @@
         </is>
       </c>
       <c r="F53" s="4" t="n">
-        <v>45756.53509356372</v>
+        <v>45757.92920302729</v>
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
@@ -2794,7 +2794,7 @@
         </is>
       </c>
       <c r="F54" s="4" t="n">
-        <v>45756.53509419255</v>
+        <v>45757.92920367206</v>
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
@@ -2837,7 +2837,7 @@
         </is>
       </c>
       <c r="F55" s="4" t="n">
-        <v>45756.53509472703</v>
+        <v>45757.92920424325</v>
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
@@ -2880,7 +2880,7 @@
         </is>
       </c>
       <c r="F56" s="4" t="n">
-        <v>45756.53509534904</v>
+        <v>45757.9292048289</v>
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
@@ -2923,7 +2923,7 @@
         </is>
       </c>
       <c r="F57" s="4" t="n">
-        <v>45756.53509592765</v>
+        <v>45757.92920534197</v>
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
@@ -2944,12 +2944,10 @@
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>windows_area_by_room_by_globalid_021YoEi1HD9eSoSLT0LMfy</t>
-        </is>
-      </c>
-      <c r="B58" s="3" t="n">
-        <v>3.0551</v>
-      </c>
+          <t>windows_external_area_by_room_by_globalid</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr"/>
       <c r="C58" s="2" t="inlineStr">
         <is>
           <t>m²</t>
@@ -2957,20 +2955,16 @@
       </c>
       <c r="D58" s="2" t="inlineStr">
         <is>
-          <t>area</t>
-        </is>
-      </c>
-      <c r="E58" s="2" t="inlineStr">
-        <is>
-          <t>Get windows grouped by room</t>
-        </is>
-      </c>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr"/>
       <c r="F58" s="4" t="n">
-        <v>45756.53509650254</v>
+        <v>45757.92920608172</v>
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>error: No results calculated</t>
         </is>
       </c>
       <c r="H58" s="2" t="inlineStr">
@@ -2987,12 +2981,10 @@
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>windows_area_by_room_by_globalid_2ky6TqzMD7gwJbHxE3Kcxy</t>
-        </is>
-      </c>
-      <c r="B59" s="3" t="n">
-        <v>3.0551</v>
-      </c>
+          <t>windows_internal_area_by_room_by_globalid</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr"/>
       <c r="C59" s="2" t="inlineStr">
         <is>
           <t>m²</t>
@@ -3000,20 +2992,16 @@
       </c>
       <c r="D59" s="2" t="inlineStr">
         <is>
-          <t>area</t>
-        </is>
-      </c>
-      <c r="E59" s="2" t="inlineStr">
-        <is>
-          <t>Get windows grouped by room</t>
-        </is>
-      </c>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr"/>
       <c r="F59" s="4" t="n">
-        <v>45756.53509650272</v>
+        <v>45757.92920667143</v>
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>error: No results calculated</t>
         </is>
       </c>
       <c r="H59" s="2" t="inlineStr">
@@ -3030,7 +3018,7 @@
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>doors_interior_area_by_room_type_by_globalid</t>
+          <t>wall_surface_net_area_by_room_type_by_longname</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr"/>
@@ -3046,7 +3034,7 @@
       </c>
       <c r="E60" s="2" t="inlineStr"/>
       <c r="F60" s="4" t="n">
-        <v>45756.53509708327</v>
+        <v>45757.92920730879</v>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
@@ -3067,11 +3055,11 @@
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>doors_exterior_area_by_room_type_by_globalid_2lk8ATQRL3YhM35IFLYXiz</t>
+          <t>room_area_by_room_type_sgr</t>
         </is>
       </c>
       <c r="B61" s="3" t="n">
-        <v>2.1</v>
+        <v>55.21875</v>
       </c>
       <c r="C61" s="2" t="inlineStr">
         <is>
@@ -3085,11 +3073,11 @@
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>Get exterior doors grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F61" s="4" t="n">
-        <v>45756.53509769844</v>
+        <v>45757.92920791926</v>
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
@@ -3110,11 +3098,11 @@
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_SGR</t>
+          <t>room_area_by_room_type_</t>
         </is>
       </c>
       <c r="B62" s="3" t="n">
-        <v>89.19</v>
+        <v>485.86955</v>
       </c>
       <c r="C62" s="2" t="inlineStr">
         <is>
@@ -3128,11 +3116,11 @@
       </c>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F62" s="4" t="n">
-        <v>45756.53509851803</v>
+        <v>45757.92920791938</v>
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
@@ -3153,11 +3141,11 @@
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_GSA</t>
+          <t>room_area_by_room_type_gsa</t>
         </is>
       </c>
       <c r="B63" s="3" t="n">
-        <v>128.1469</v>
+        <v>35.9925</v>
       </c>
       <c r="C63" s="2" t="inlineStr">
         <is>
@@ -3171,11 +3159,11 @@
       </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F63" s="4" t="n">
-        <v>45756.53509851833</v>
+        <v>45757.9292079194</v>
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
@@ -3196,11 +3184,11 @@
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_TRH</t>
+          <t>room_area_by_room_type_trh</t>
         </is>
       </c>
       <c r="B64" s="3" t="n">
-        <v>100.0458</v>
+        <v>34.88275</v>
       </c>
       <c r="C64" s="2" t="inlineStr">
         <is>
@@ -3214,11 +3202,11 @@
       </c>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F64" s="4" t="n">
-        <v>45756.53509851839</v>
+        <v>45757.92920791941</v>
       </c>
       <c r="G64" s="2" t="inlineStr">
         <is>
@@ -3239,11 +3227,11 @@
     <row r="65">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_LUF</t>
+          <t>room_area_by_room_type_buf</t>
         </is>
       </c>
       <c r="B65" s="3" t="n">
-        <v>32.205</v>
+        <v>153.643603</v>
       </c>
       <c r="C65" s="2" t="inlineStr">
         <is>
@@ -3257,11 +3245,11 @@
       </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F65" s="4" t="n">
-        <v>45756.53509851847</v>
+        <v>45757.92920791942</v>
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
@@ -3282,11 +3270,11 @@
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_WCH</t>
+          <t>room_area_by_room_type_uuf</t>
         </is>
       </c>
       <c r="B66" s="3" t="n">
-        <v>38.94</v>
+        <v>78.724515</v>
       </c>
       <c r="C66" s="2" t="inlineStr">
         <is>
@@ -3300,11 +3288,11 @@
       </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F66" s="4" t="n">
-        <v>45756.53509851853</v>
+        <v>45757.92920791943</v>
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
@@ -3325,11 +3313,11 @@
     <row r="67">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_WCD</t>
+          <t>room_area_by_room_type_luf</t>
         </is>
       </c>
       <c r="B67" s="3" t="n">
-        <v>38.94</v>
+        <v>11.625</v>
       </c>
       <c r="C67" s="2" t="inlineStr">
         <is>
@@ -3343,11 +3331,11 @@
       </c>
       <c r="E67" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F67" s="4" t="n">
-        <v>45756.53509851858</v>
+        <v>45757.92920791944</v>
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
@@ -3368,11 +3356,11 @@
     <row r="68">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>wall_surface_net_area_by_room_type_by_longname_RRG</t>
+          <t>room_area_by_room_type_vrf</t>
         </is>
       </c>
       <c r="B68" s="3" t="n">
-        <v>38.94</v>
+        <v>15.5</v>
       </c>
       <c r="C68" s="2" t="inlineStr">
         <is>
@@ -3386,11 +3374,11 @@
       </c>
       <c r="E68" s="2" t="inlineStr">
         <is>
-          <t>Get wall coverings grouped by room</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F68" s="4" t="n">
-        <v>45756.53509851866</v>
+        <v>45757.92920791951</v>
       </c>
       <c r="G68" s="2" t="inlineStr">
         <is>
@@ -3411,11 +3399,11 @@
     <row r="69">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>facade_net_area_by_direction_180</t>
+          <t>room_area_by_room_type_wch</t>
         </is>
       </c>
       <c r="B69" s="3" t="n">
-        <v>90.70567000001473</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2" t="inlineStr">
         <is>
@@ -3429,11 +3417,11 @@
       </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
-          <t>Get facade gross area grouped by direction</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F69" s="4" t="n">
-        <v>45756.53509937542</v>
+        <v>45757.92920791954</v>
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
@@ -3454,11 +3442,11 @@
     <row r="70">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>facade_net_area_by_direction_90</t>
+          <t>room_area_by_room_type_wcd</t>
         </is>
       </c>
       <c r="B70" s="3" t="n">
-        <v>92.47996601016342</v>
+        <v>10</v>
       </c>
       <c r="C70" s="2" t="inlineStr">
         <is>
@@ -3472,11 +3460,11 @@
       </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>Get facade gross area grouped by direction</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F70" s="4" t="n">
-        <v>45756.53509937577</v>
+        <v>45757.92920791955</v>
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
@@ -3497,11 +3485,11 @@
     <row r="71">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>facade_net_area_by_direction_0</t>
+          <t>room_area_by_room_type_rrg</t>
         </is>
       </c>
       <c r="B71" s="3" t="n">
-        <v>94.75418799999998</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2" t="inlineStr">
         <is>
@@ -3515,11 +3503,11 @@
       </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
-          <t>Get facade gross area grouped by direction</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F71" s="4" t="n">
-        <v>45756.53509937583</v>
+        <v>45757.92920791956</v>
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
@@ -3540,11 +3528,11 @@
     <row r="72">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>facade_net_area_by_direction_-90</t>
+          <t>room_area_by_room_type_flachdach</t>
         </is>
       </c>
       <c r="B72" s="3" t="n">
-        <v>85.8115</v>
+        <v>73.80325000000001</v>
       </c>
       <c r="C72" s="2" t="inlineStr">
         <is>
@@ -3558,11 +3546,11 @@
       </c>
       <c r="E72" s="2" t="inlineStr">
         <is>
-          <t>Get facade gross area grouped by direction</t>
+          <t>Get room area grouped by room type</t>
         </is>
       </c>
       <c r="F72" s="4" t="n">
-        <v>45756.53509937588</v>
+        <v>45757.92920791957</v>
       </c>
       <c r="G72" s="2" t="inlineStr">
         <is>
@@ -3583,11 +3571,11 @@
     <row r="73">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>windows_area_by_direction_180</t>
+          <t>room_volume_by_room_type_sgr</t>
         </is>
       </c>
       <c r="B73" s="3" t="n">
-        <v>6.1102</v>
+        <v>165.65625</v>
       </c>
       <c r="C73" s="2" t="inlineStr">
         <is>
@@ -3601,11 +3589,11 @@
       </c>
       <c r="E73" s="2" t="inlineStr">
         <is>
-          <t>Get windows area grouped by direction</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F73" s="4" t="n">
-        <v>45756.53510002307</v>
+        <v>45757.92920851232</v>
       </c>
       <c r="G73" s="2" t="inlineStr">
         <is>
@@ -3626,11 +3614,11 @@
     <row r="74">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>construction_area</t>
+          <t>room_volume_by_room_type_</t>
         </is>
       </c>
       <c r="B74" s="3" t="n">
-        <v>38.32</v>
+        <v>916.2459050000001</v>
       </c>
       <c r="C74" s="2" t="inlineStr">
         <is>
@@ -3644,11 +3632,11 @@
       </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
-          <t>gross_floor_area - space_interior_floor_area</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F74" s="4" t="n">
-        <v>45756.53510026188</v>
+        <v>45757.92920851244</v>
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
@@ -3669,11 +3657,11 @@
     <row r="75">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>construction_area_above_ground</t>
+          <t>room_volume_by_room_type_gsa</t>
         </is>
       </c>
       <c r="B75" s="3" t="n">
-        <v>27.41</v>
+        <v>107.9775</v>
       </c>
       <c r="C75" s="2" t="inlineStr">
         <is>
@@ -3687,11 +3675,11 @@
       </c>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>gross_floor_area_above_ground - space_interior_floor_area_above_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F75" s="4" t="n">
-        <v>45756.53510028996</v>
+        <v>45757.92920851245</v>
       </c>
       <c r="G75" s="2" t="inlineStr">
         <is>
@@ -3712,11 +3700,11 @@
     <row r="76">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>construction_area_below_ground</t>
+          <t>room_volume_by_room_type_trh</t>
         </is>
       </c>
       <c r="B76" s="3" t="n">
-        <v>10.9</v>
+        <v>113.95135</v>
       </c>
       <c r="C76" s="2" t="inlineStr">
         <is>
@@ -3730,11 +3718,11 @@
       </c>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>gross_floor_area_below_ground - space_interior_floor_area_below_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F76" s="4" t="n">
-        <v>45756.5351003123</v>
+        <v>45757.92920851247</v>
       </c>
       <c r="G76" s="2" t="inlineStr">
         <is>
@@ -3755,29 +3743,29 @@
     <row r="77">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>construction_volume</t>
+          <t>room_volume_by_room_type_buf</t>
         </is>
       </c>
       <c r="B77" s="3" t="n">
-        <v>197.75</v>
+        <v>153.643603</v>
       </c>
       <c r="C77" s="2" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
-          <t>gross_volume - space_interior_volume</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F77" s="4" t="n">
-        <v>45756.53510033507</v>
+        <v>45757.92920851249</v>
       </c>
       <c r="G77" s="2" t="inlineStr">
         <is>
@@ -3798,29 +3786,29 @@
     <row r="78">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_above_ground</t>
+          <t>room_volume_by_room_type_uuf</t>
         </is>
       </c>
       <c r="B78" s="3" t="n">
-        <v>105.54</v>
+        <v>78.724515</v>
       </c>
       <c r="C78" s="2" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D78" s="2" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>gross_volume_above_ground - space_interior_volume_above_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F78" s="4" t="n">
-        <v>45756.53510035505</v>
+        <v>45757.9292085125</v>
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
@@ -3841,29 +3829,29 @@
     <row r="79">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_below_ground</t>
+          <t>room_volume_by_room_type_luf</t>
         </is>
       </c>
       <c r="B79" s="3" t="n">
-        <v>92.20999999999999</v>
+        <v>34.875</v>
       </c>
       <c r="C79" s="2" t="inlineStr">
         <is>
-          <t>m³</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D79" s="2" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
-          <t>gross_volume_below_ground - space_interior_volume_below_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F79" s="4" t="n">
-        <v>45756.53510037693</v>
+        <v>45757.92920851251</v>
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
@@ -3884,29 +3872,29 @@
     <row r="80">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>gv_to_gf_ratio</t>
+          <t>room_volume_by_room_type_vrf</t>
         </is>
       </c>
       <c r="B80" s="3" t="n">
-        <v>3.65</v>
+        <v>15.5</v>
       </c>
       <c r="C80" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D80" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E80" s="2" t="inlineStr">
         <is>
-          <t>gross_volume / gross_floor_area</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F80" s="4" t="n">
-        <v>45756.53510039656</v>
+        <v>45757.92920851252</v>
       </c>
       <c r="G80" s="2" t="inlineStr">
         <is>
@@ -3927,29 +3915,29 @@
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>window_to_floor_ratio</t>
+          <t>room_volume_by_room_type_wch</t>
         </is>
       </c>
       <c r="B81" s="3" t="n">
-        <v>0.03</v>
+        <v>30</v>
       </c>
       <c r="C81" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D81" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
-          <t>windows_exterior_area / gross_floor_area</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F81" s="4" t="n">
-        <v>45756.53510041917</v>
+        <v>45757.92920851253</v>
       </c>
       <c r="G81" s="2" t="inlineStr">
         <is>
@@ -3970,29 +3958,29 @@
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_volume_ratio</t>
+          <t>room_volume_by_room_type_wcd</t>
         </is>
       </c>
       <c r="B82" s="3" t="n">
-        <v>0.52</v>
+        <v>30</v>
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>(facade_vertical_area + windows_exterior_area + doors_exterior_area) / gross_volume</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F82" s="4" t="n">
-        <v>45756.53510043881</v>
+        <v>45757.92920851255</v>
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
@@ -4013,29 +4001,29 @@
     <row r="83">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_volume_ratio_above_ground</t>
+          <t>room_volume_by_room_type_rrg</t>
         </is>
       </c>
       <c r="B83" s="3" t="n">
-        <v>0.57</v>
+        <v>30</v>
       </c>
       <c r="C83" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E83" s="2" t="inlineStr">
         <is>
-          <t>(facade_vertical_area_above_ground + windows_exterior_area_above_ground + doors_exterior_area_above_ground) / gross_volume_above_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F83" s="4" t="n">
-        <v>45756.53510045834</v>
+        <v>45757.92920851256</v>
       </c>
       <c r="G83" s="2" t="inlineStr">
         <is>
@@ -4056,29 +4044,29 @@
     <row r="84">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_volume_ratio_below_ground</t>
+          <t>room_volume_by_room_type_flachdach</t>
         </is>
       </c>
       <c r="B84" s="3" t="n">
-        <v>0.44</v>
+        <v>73.80325000000001</v>
       </c>
       <c r="C84" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E84" s="2" t="inlineStr">
         <is>
-          <t>(facade_vertical_area_below_ground + windows_exterior_area_below_ground + doors_exterior_area_below_ground) / gross_volume_below_ground</t>
+          <t>Get room volume grouped by room type</t>
         </is>
       </c>
       <c r="F84" s="4" t="n">
-        <v>45756.53510047957</v>
+        <v>45757.92920851258</v>
       </c>
       <c r="G84" s="2" t="inlineStr">
         <is>
@@ -4099,33 +4087,27 @@
     <row r="85">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_floor_area_ratio</t>
-        </is>
-      </c>
-      <c r="B85" s="3" t="n">
-        <v>1.91</v>
-      </c>
+          <t>facade_net_area_by_direction</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr"/>
       <c r="C85" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D85" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
-        </is>
-      </c>
-      <c r="E85" s="2" t="inlineStr">
-        <is>
-          <t>(facade_vertical_area + windows_exterior_area + doors_exterior_area) / gross_floor_area</t>
-        </is>
-      </c>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="E85" s="2" t="inlineStr"/>
       <c r="F85" s="4" t="n">
-        <v>45756.53510049904</v>
+        <v>45757.92920976316</v>
       </c>
       <c r="G85" s="2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>error: No results calculated</t>
         </is>
       </c>
       <c r="H85" s="2" t="inlineStr">
@@ -4142,33 +4124,27 @@
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_floor_area_ratio_above_ground</t>
-        </is>
-      </c>
-      <c r="B86" s="3" t="n">
-        <v>1.33</v>
-      </c>
+          <t>windows_area_by_direction</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr"/>
       <c r="C86" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D86" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
-        </is>
-      </c>
-      <c r="E86" s="2" t="inlineStr">
-        <is>
-          <t>(facade_vertical_area_above_ground + windows_exterior_area_above_ground + doors_exterior_area_above_ground) / gross_floor_area</t>
-        </is>
-      </c>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="E86" s="2" t="inlineStr"/>
       <c r="F86" s="4" t="n">
-        <v>45756.53510052</v>
+        <v>45757.92921032613</v>
       </c>
       <c r="G86" s="2" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>error: No results calculated</t>
         </is>
       </c>
       <c r="H86" s="2" t="inlineStr">
@@ -4185,29 +4161,29 @@
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>facade_area_to_gross_floor_area_ratio_below_ground</t>
+          <t>construction_area</t>
         </is>
       </c>
       <c r="B87" s="3" t="n">
-        <v>0.59</v>
+        <v>49.95</v>
       </c>
       <c r="C87" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D87" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
-          <t>(facade_vertical_area_below_ground + windows_exterior_area_below_ground + doors_exterior_area_below_ground) / gross_floor_area</t>
+          <t>gross_floor_area - space_interior_floor_area</t>
         </is>
       </c>
       <c r="F87" s="4" t="n">
-        <v>45756.53510053897</v>
+        <v>45757.92921055241</v>
       </c>
       <c r="G87" s="2" t="inlineStr">
         <is>
@@ -4228,29 +4204,29 @@
     <row r="88">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>windows_area_to_total_facade_area_ratio</t>
+          <t>construction_area_above_ground</t>
         </is>
       </c>
       <c r="B88" s="3" t="n">
-        <v>0.02</v>
+        <v>39.04</v>
       </c>
       <c r="C88" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D88" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E88" s="2" t="inlineStr">
         <is>
-          <t>windows_exterior_area / facade_vertical_area</t>
+          <t>gross_floor_area_above_ground - space_interior_floor_area_above_ground</t>
         </is>
       </c>
       <c r="F88" s="4" t="n">
-        <v>45756.53510055772</v>
+        <v>45757.92921057555</v>
       </c>
       <c r="G88" s="2" t="inlineStr">
         <is>
@@ -4271,29 +4247,29 @@
     <row r="89">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>windows_area_to_total_facade_area_ratio_above_ground</t>
+          <t>construction_area_below_ground</t>
         </is>
       </c>
       <c r="B89" s="3" t="n">
-        <v>0.02</v>
+        <v>10.9</v>
       </c>
       <c r="C89" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m²</t>
         </is>
       </c>
       <c r="D89" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>area</t>
         </is>
       </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
-          <t>windows_exterior_area_above_ground / facade_vertical_area_above_ground</t>
+          <t>gross_floor_area_below_ground - space_interior_floor_area_below_ground</t>
         </is>
       </c>
       <c r="F89" s="4" t="n">
-        <v>45756.5351005784</v>
+        <v>45757.92921059558</v>
       </c>
       <c r="G89" s="2" t="inlineStr">
         <is>
@@ -4314,29 +4290,29 @@
     <row r="90">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>windows_area_to_total_facade_area_ratio_below_ground</t>
+          <t>construction_volume</t>
         </is>
       </c>
       <c r="B90" s="3" t="n">
-        <v>0</v>
+        <v>197.75</v>
       </c>
       <c r="C90" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="D90" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>volume</t>
         </is>
       </c>
       <c r="E90" s="2" t="inlineStr">
         <is>
-          <t>windows_exterior_area_below_ground / facade_vertical_area_below_ground</t>
+          <t>gross_volume - space_interior_volume</t>
         </is>
       </c>
       <c r="F90" s="4" t="n">
-        <v>45756.53510059713</v>
+        <v>45757.92921061573</v>
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
@@ -4357,29 +4333,29 @@
     <row r="91">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>construction_area_to_gross_floor_area_ratio</t>
+          <t>construction_volume_above_ground</t>
         </is>
       </c>
       <c r="B91" s="3" t="n">
-        <v>0.2</v>
+        <v>105.54</v>
       </c>
       <c r="C91" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="D91" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>volume</t>
         </is>
       </c>
       <c r="E91" s="2" t="inlineStr">
         <is>
-          <t>construction_area / gross_floor_area</t>
+          <t>gross_volume_above_ground - space_interior_volume_above_ground</t>
         </is>
       </c>
       <c r="F91" s="4" t="n">
-        <v>45756.53510061769</v>
+        <v>45757.929210635</v>
       </c>
       <c r="G91" s="2" t="inlineStr">
         <is>
@@ -4400,29 +4376,29 @@
     <row r="92">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>construction_area_to_gross_floor_area_ratio_above_ground</t>
+          <t>construction_volume_below_ground</t>
         </is>
       </c>
       <c r="B92" s="3" t="n">
-        <v>0.14</v>
+        <v>92.20999999999999</v>
       </c>
       <c r="C92" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>m³</t>
         </is>
       </c>
       <c r="D92" s="2" t="inlineStr">
         <is>
-          <t>ratio</t>
+          <t>volume</t>
         </is>
       </c>
       <c r="E92" s="2" t="inlineStr">
         <is>
-          <t>construction_area_above_ground / gross_floor_area</t>
+          <t>gross_volume_below_ground - space_interior_volume_below_ground</t>
         </is>
       </c>
       <c r="F92" s="4" t="n">
-        <v>45756.53510063673</v>
+        <v>45757.92921065429</v>
       </c>
       <c r="G92" s="2" t="inlineStr">
         <is>
@@ -4443,11 +4419,11 @@
     <row r="93">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>construction_area_to_gross_floor_area_ratio_below_ground</t>
+          <t>gv_to_gf_ratio</t>
         </is>
       </c>
       <c r="B93" s="3" t="n">
-        <v>0.06</v>
+        <v>3.45</v>
       </c>
       <c r="C93" s="2" t="inlineStr">
         <is>
@@ -4461,11 +4437,11 @@
       </c>
       <c r="E93" s="2" t="inlineStr">
         <is>
-          <t>construction_area_below_ground / gross_floor_area</t>
+          <t>gross_volume / gross_floor_area</t>
         </is>
       </c>
       <c r="F93" s="4" t="n">
-        <v>45756.53510065722</v>
+        <v>45757.92921067338</v>
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
@@ -4486,11 +4462,11 @@
     <row r="94">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_to_gross_volume_ratio</t>
+          <t>window_to_floor_ratio</t>
         </is>
       </c>
       <c r="B94" s="3" t="n">
-        <v>0.28</v>
+        <v>0.03</v>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
@@ -4504,11 +4480,11 @@
       </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
-          <t>construction_volume / gross_volume</t>
+          <t>windows_exterior_area / gross_floor_area</t>
         </is>
       </c>
       <c r="F94" s="4" t="n">
-        <v>45756.53510067554</v>
+        <v>45757.92921069371</v>
       </c>
       <c r="G94" s="2" t="inlineStr">
         <is>
@@ -4529,11 +4505,11 @@
     <row r="95">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_to_gross_volume_ratio_above_ground</t>
+          <t>facade_area_to_gross_volume_ratio</t>
         </is>
       </c>
       <c r="B95" s="3" t="n">
-        <v>0.23</v>
+        <v>0.52</v>
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
@@ -4547,11 +4523,11 @@
       </c>
       <c r="E95" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_above_ground / gross_volume_above_ground</t>
+          <t>(facade_vertical_area + windows_exterior_area + doors_exterior_area) / gross_volume</t>
         </is>
       </c>
       <c r="F95" s="4" t="n">
-        <v>45756.53510069457</v>
+        <v>45757.92921071288</v>
       </c>
       <c r="G95" s="2" t="inlineStr">
         <is>
@@ -4572,11 +4548,11 @@
     <row r="96">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_to_gross_volume_ratio_below_ground</t>
+          <t>facade_area_to_gross_volume_ratio_above_ground</t>
         </is>
       </c>
       <c r="B96" s="3" t="n">
-        <v>0.36</v>
+        <v>0.57</v>
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
@@ -4590,11 +4566,11 @@
       </c>
       <c r="E96" s="2" t="inlineStr">
         <is>
-          <t>construction_volume_below_ground / gross_volume_below_ground</t>
+          <t>(facade_vertical_area_above_ground + windows_exterior_area_above_ground + doors_exterior_area_above_ground) / gross_volume_above_ground</t>
         </is>
       </c>
       <c r="F96" s="4" t="n">
-        <v>45756.53510071507</v>
+        <v>45757.92921073172</v>
       </c>
       <c r="G96" s="2" t="inlineStr">
         <is>
@@ -4615,29 +4591,29 @@
     <row r="97">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>total_envelope_area</t>
+          <t>facade_area_to_gross_volume_ratio_below_ground</t>
         </is>
       </c>
       <c r="B97" s="3" t="n">
-        <v>552.39</v>
+        <v>0.44</v>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>m²</t>
+          <t>ratio</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
         <is>
-          <t>area</t>
+          <t>ratio</t>
         </is>
       </c>
       <c r="E97" s="2" t="inlineStr">
         <is>
-          <t>facade_vertical_area + windows_exterior_area + doors_exterior_area + roof_area + soffit_area</t>
+          <t>(facade_vertical_area_below_ground + windows_exterior_area_below_ground + doors_exterior_area_below_ground) / gross_volume_below_ground</t>
         </is>
       </c>
       <c r="F97" s="4" t="n">
-        <v>45756.53510073393</v>
+        <v>45757.92921075042</v>
       </c>
       <c r="G97" s="2" t="inlineStr">
         <is>
@@ -4658,11 +4634,11 @@
     <row r="98">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>total_envelope_area_to_gross_floor_area_ratio</t>
+          <t>facade_area_to_gross_floor_area_ratio</t>
         </is>
       </c>
       <c r="B98" s="3" t="n">
-        <v>2.84</v>
+        <v>1.81</v>
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
@@ -4676,11 +4652,11 @@
       </c>
       <c r="E98" s="2" t="inlineStr">
         <is>
-          <t>total_envelope_area / gross_floor_area</t>
+          <t>(facade_vertical_area + windows_exterior_area + doors_exterior_area) / gross_floor_area</t>
         </is>
       </c>
       <c r="F98" s="4" t="n">
-        <v>45756.53510075441</v>
+        <v>45757.92921076916</v>
       </c>
       <c r="G98" s="2" t="inlineStr">
         <is>
@@ -4701,11 +4677,11 @@
     <row r="99">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>total_envelope_area_to_gross_volume_ratio</t>
+          <t>facade_area_to_gross_floor_area_ratio_above_ground</t>
         </is>
       </c>
       <c r="B99" s="3" t="n">
-        <v>0.78</v>
+        <v>1.25</v>
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
@@ -4719,11 +4695,11 @@
       </c>
       <c r="E99" s="2" t="inlineStr">
         <is>
-          <t>total_envelope_area / gross_volume</t>
+          <t>(facade_vertical_area_above_ground + windows_exterior_area_above_ground + doors_exterior_area_above_ground) / gross_floor_area</t>
         </is>
       </c>
       <c r="F99" s="4" t="n">
-        <v>45756.53510077296</v>
+        <v>45757.92921078808</v>
       </c>
       <c r="G99" s="2" t="inlineStr">
         <is>
@@ -4744,29 +4720,29 @@
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>storeys_count_excluding_roof</t>
+          <t>facade_area_to_gross_floor_area_ratio_below_ground</t>
         </is>
       </c>
       <c r="B100" s="3" t="n">
-        <v>4</v>
+        <v>0.55</v>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>ratio</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
         <is>
-          <t>count</t>
+          <t>ratio</t>
         </is>
       </c>
       <c r="E100" s="2" t="inlineStr">
         <is>
-          <t>storeys_count_including_roof - 1</t>
+          <t>(facade_vertical_area_below_ground + windows_exterior_area_below_ground + doors_exterior_area_below_ground) / gross_floor_area</t>
         </is>
       </c>
       <c r="F100" s="4" t="n">
-        <v>45756.53510079163</v>
+        <v>45757.92921080678</v>
       </c>
       <c r="G100" s="2" t="inlineStr">
         <is>
@@ -4787,41 +4763,600 @@
     <row r="101">
       <c r="A101" s="2" t="inlineStr">
         <is>
+          <t>windows_area_to_total_facade_area_ratio</t>
+        </is>
+      </c>
+      <c r="B101" s="3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C101" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E101" s="2" t="inlineStr">
+        <is>
+          <t>windows_exterior_area / facade_vertical_area</t>
+        </is>
+      </c>
+      <c r="F101" s="4" t="n">
+        <v>45757.92921082522</v>
+      </c>
+      <c r="G101" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H101" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I101" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>windows_area_to_total_facade_area_ratio_above_ground</t>
+        </is>
+      </c>
+      <c r="B102" s="3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E102" s="2" t="inlineStr">
+        <is>
+          <t>windows_exterior_area_above_ground / facade_vertical_area_above_ground</t>
+        </is>
+      </c>
+      <c r="F102" s="4" t="n">
+        <v>45757.92921084368</v>
+      </c>
+      <c r="G102" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H102" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I102" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="inlineStr">
+        <is>
+          <t>windows_area_to_total_facade_area_ratio_below_ground</t>
+        </is>
+      </c>
+      <c r="B103" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C103" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D103" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E103" s="2" t="inlineStr">
+        <is>
+          <t>windows_exterior_area_below_ground / facade_vertical_area_below_ground</t>
+        </is>
+      </c>
+      <c r="F103" s="4" t="n">
+        <v>45757.92921086233</v>
+      </c>
+      <c r="G103" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H103" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I103" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>construction_area_to_gross_floor_area_ratio</t>
+        </is>
+      </c>
+      <c r="B104" s="3" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E104" s="2" t="inlineStr">
+        <is>
+          <t>construction_area / gross_floor_area</t>
+        </is>
+      </c>
+      <c r="F104" s="4" t="n">
+        <v>45757.92921088088</v>
+      </c>
+      <c r="G104" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H104" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I104" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="inlineStr">
+        <is>
+          <t>construction_area_to_gross_floor_area_ratio_above_ground</t>
+        </is>
+      </c>
+      <c r="B105" s="3" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="C105" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E105" s="2" t="inlineStr">
+        <is>
+          <t>construction_area_above_ground / gross_floor_area</t>
+        </is>
+      </c>
+      <c r="F105" s="4" t="n">
+        <v>45757.92921089938</v>
+      </c>
+      <c r="G105" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H105" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I105" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>construction_area_to_gross_floor_area_ratio_below_ground</t>
+        </is>
+      </c>
+      <c r="B106" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E106" s="2" t="inlineStr">
+        <is>
+          <t>construction_area_below_ground / gross_floor_area</t>
+        </is>
+      </c>
+      <c r="F106" s="4" t="n">
+        <v>45757.92921091802</v>
+      </c>
+      <c r="G106" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H106" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I106" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume_to_gross_volume_ratio</t>
+        </is>
+      </c>
+      <c r="B107" s="3" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="C107" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D107" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E107" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume / gross_volume</t>
+        </is>
+      </c>
+      <c r="F107" s="4" t="n">
+        <v>45757.92921093635</v>
+      </c>
+      <c r="G107" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H107" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I107" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume_to_gross_volume_ratio_above_ground</t>
+        </is>
+      </c>
+      <c r="B108" s="3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="C108" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D108" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E108" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume_above_ground / gross_volume_above_ground</t>
+        </is>
+      </c>
+      <c r="F108" s="4" t="n">
+        <v>45757.92921095521</v>
+      </c>
+      <c r="G108" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H108" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I108" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume_to_gross_volume_ratio_below_ground</t>
+        </is>
+      </c>
+      <c r="B109" s="3" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="C109" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D109" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E109" s="2" t="inlineStr">
+        <is>
+          <t>construction_volume_below_ground / gross_volume_below_ground</t>
+        </is>
+      </c>
+      <c r="F109" s="4" t="n">
+        <v>45757.92921097356</v>
+      </c>
+      <c r="G109" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H109" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I109" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="inlineStr">
+        <is>
+          <t>total_envelope_area</t>
+        </is>
+      </c>
+      <c r="B110" s="3" t="n">
+        <v>552.39</v>
+      </c>
+      <c r="C110" s="2" t="inlineStr">
+        <is>
+          <t>m²</t>
+        </is>
+      </c>
+      <c r="D110" s="2" t="inlineStr">
+        <is>
+          <t>area</t>
+        </is>
+      </c>
+      <c r="E110" s="2" t="inlineStr">
+        <is>
+          <t>facade_vertical_area + windows_exterior_area + doors_exterior_area + roof_area + soffit_area</t>
+        </is>
+      </c>
+      <c r="F110" s="4" t="n">
+        <v>45757.92921099238</v>
+      </c>
+      <c r="G110" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H110" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I110" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="inlineStr">
+        <is>
+          <t>total_envelope_area_to_gross_floor_area_ratio</t>
+        </is>
+      </c>
+      <c r="B111" s="3" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="C111" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E111" s="2" t="inlineStr">
+        <is>
+          <t>total_envelope_area / gross_floor_area</t>
+        </is>
+      </c>
+      <c r="F111" s="4" t="n">
+        <v>45757.92921101145</v>
+      </c>
+      <c r="G111" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H111" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I111" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="inlineStr">
+        <is>
+          <t>total_envelope_area_to_gross_volume_ratio</t>
+        </is>
+      </c>
+      <c r="B112" s="3" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="C112" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="D112" s="2" t="inlineStr">
+        <is>
+          <t>ratio</t>
+        </is>
+      </c>
+      <c r="E112" s="2" t="inlineStr">
+        <is>
+          <t>total_envelope_area / gross_volume</t>
+        </is>
+      </c>
+      <c r="F112" s="4" t="n">
+        <v>45757.92921103055</v>
+      </c>
+      <c r="G112" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H112" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I112" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="inlineStr">
+        <is>
+          <t>storeys_count_excluding_roof</t>
+        </is>
+      </c>
+      <c r="B113" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C113" s="2" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="D113" s="2" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+      <c r="E113" s="2" t="inlineStr">
+        <is>
+          <t>storeys_count_including_roof - 1</t>
+        </is>
+      </c>
+      <c r="F113" s="4" t="n">
+        <v>45757.92921104912</v>
+      </c>
+      <c r="G113" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H113" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I113" s="2" t="inlineStr">
+        <is>
+          <t>IFC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="inlineStr">
+        <is>
           <t>storeys_count_excluding_roof_above_ground</t>
         </is>
       </c>
-      <c r="B101" s="3" t="n">
+      <c r="B114" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="C101" s="2" t="inlineStr">
+      <c r="C114" s="2" t="inlineStr">
         <is>
           <t>count</t>
         </is>
       </c>
-      <c r="D101" s="2" t="inlineStr">
+      <c r="D114" s="2" t="inlineStr">
         <is>
           <t>count</t>
         </is>
       </c>
-      <c r="E101" s="2" t="inlineStr">
+      <c r="E114" s="2" t="inlineStr">
         <is>
           <t>storeys_count_including_roof_above_ground - 1</t>
         </is>
       </c>
-      <c r="F101" s="4" t="n">
-        <v>45756.53510081182</v>
-      </c>
-      <c r="G101" s="2" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="H101" s="2" t="inlineStr">
-        <is>
-          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
-        </is>
-      </c>
-      <c r="I101" s="2" t="inlineStr">
+      <c r="F114" s="4" t="n">
+        <v>45757.92921106898</v>
+      </c>
+      <c r="G114" s="2" t="inlineStr">
+        <is>
+          <t>success</t>
+        </is>
+      </c>
+      <c r="H114" s="2" t="inlineStr">
+        <is>
+          <t>Mustermodell V1_abstractBIM_sp_enriched.ifc</t>
+        </is>
+      </c>
+      <c r="I114" s="2" t="inlineStr">
         <is>
           <t>IFC4</t>
         </is>

</xml_diff>